<commit_message>
updated with more products
</commit_message>
<xml_diff>
--- a/db/db_setup.xlsx
+++ b/db/db_setup.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham_vickers/Documents/sportchek_cms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham_vickers/Documents/sportchek_cms/db/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B41A84-6604-1149-A217-0298E710EE49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CA53105-EB68-A842-9F81-FDADB0A91209}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16920" yWindow="0" windowWidth="16680" windowHeight="21000" xr2:uid="{A04C6813-D711-3940-89A1-E6A3A85ADC53}"/>
+    <workbookView xWindow="32200" yWindow="0" windowWidth="19000" windowHeight="21600" xr2:uid="{A04C6813-D711-3940-89A1-E6A3A85ADC53}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t>prod_id</t>
   </si>
@@ -363,6 +363,33 @@
   </si>
   <si>
     <t>columbia_skirt.png</t>
+  </si>
+  <si>
+    <t>Nike Hoodie - Womens - Blue</t>
+  </si>
+  <si>
+    <t>Loosen up in the Nike Sportswear Essential Women's Fleece Pullover Hoodie, your go-to sweatshirt for all-day comfort.</t>
+  </si>
+  <si>
+    <t>nike_hoodie_blue.png</t>
+  </si>
+  <si>
+    <t>Under Armour - Womens - Black</t>
+  </si>
+  <si>
+    <t>A vintage old-school feel, this colourblock sweatshirt is tailored from supersoft cotton-blend fleece fabric.</t>
+  </si>
+  <si>
+    <t>ua_crewneck.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fila Hoodie - Women - Navy </t>
+  </si>
+  <si>
+    <t>From the Heritage Collection. Featuring a haphazard aesthetic, this premium sweatshirt features a reversed-out appliqué patch with a printed FILA logo.</t>
+  </si>
+  <si>
+    <t>fila_hoodie.png</t>
   </si>
 </sst>
 </file>
@@ -781,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B9AD692-76E3-E74B-9E10-80AFFAED4F29}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="81" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1017,25 +1044,25 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="D10" s="6">
-        <v>34.99</v>
+        <v>74</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>107</v>
       </c>
       <c r="F10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H10" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -1043,22 +1070,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>108</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>109</v>
       </c>
       <c r="D11" s="6">
-        <v>34.99</v>
+        <v>70</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>110</v>
       </c>
       <c r="F11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" s="1">
         <v>4</v>
@@ -1069,22 +1096,22 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>111</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="D12" s="6">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="E12" t="s">
-        <v>38</v>
+        <v>113</v>
       </c>
       <c r="F12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H12" s="1">
         <v>3</v>
@@ -1095,16 +1122,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D13" s="6">
-        <v>35</v>
+        <v>34.99</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="F13" s="1">
         <v>1</v>
@@ -1113,7 +1140,7 @@
         <v>1</v>
       </c>
       <c r="H13" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:8">
@@ -1121,19 +1148,19 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D14" s="6">
-        <v>32</v>
+        <v>34.99</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1">
         <v>1</v>
@@ -1147,25 +1174,25 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D15" s="6">
-        <v>29.95</v>
+        <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="1">
         <v>1</v>
       </c>
       <c r="H15" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:8">
@@ -1173,19 +1200,19 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D16" s="6">
         <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="F16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G16" s="1">
         <v>1</v>
@@ -1199,16 +1226,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C17" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D17" s="6">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="F17" s="1">
         <v>0</v>
@@ -1225,25 +1252,25 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="D18" s="6">
-        <v>120</v>
+        <v>29.95</v>
       </c>
       <c r="E18" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F18" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -1251,25 +1278,25 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="D19" s="6">
-        <v>110</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="F19" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H19" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -1277,25 +1304,25 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D20" s="6">
-        <v>110</v>
+        <v>55</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:8">
@@ -1303,16 +1330,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D21" s="6">
         <v>120</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F21" s="1">
         <v>1</v>
@@ -1321,7 +1348,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:8">
@@ -1329,16 +1356,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="D22" s="6">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F22" s="1">
         <v>1</v>
@@ -1355,25 +1382,25 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D23" s="6">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="F23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G23" s="1">
         <v>3</v>
       </c>
       <c r="H23" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:8">
@@ -1381,19 +1408,19 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D24" s="6">
-        <v>250</v>
+        <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="F24" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="1">
         <v>3</v>
@@ -1407,25 +1434,25 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D25" s="6">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="F25" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25" s="1">
         <v>3</v>
       </c>
       <c r="H25" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:8">
@@ -1433,16 +1460,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D26" s="6">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E26" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="F26" s="1">
         <v>0</v>
@@ -1451,7 +1478,7 @@
         <v>3</v>
       </c>
       <c r="H26" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:8">
@@ -1459,22 +1486,22 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="D27" s="6">
-        <v>48</v>
+        <v>250</v>
       </c>
       <c r="E27" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="F27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H27" s="1">
         <v>4</v>
@@ -1485,25 +1512,25 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="D28" s="6">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="E28" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G28" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H28" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:8">
@@ -1511,25 +1538,25 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C29" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D29" s="6">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="F29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G29" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H29" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="1:8">
@@ -1537,16 +1564,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D30" s="6">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F30" s="1">
         <v>1</v>
@@ -1555,24 +1582,24 @@
         <v>4</v>
       </c>
       <c r="H30" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" ht="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>84</v>
       </c>
       <c r="D31" s="6">
-        <v>89.99</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="F31" s="1">
         <v>1</v>
@@ -1589,16 +1616,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D32" s="6">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E32" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="F32" s="1">
         <v>1</v>
@@ -1607,7 +1634,7 @@
         <v>4</v>
       </c>
       <c r="H32" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -1615,16 +1642,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C33" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="D33" s="6">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E33" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="F33" s="1">
         <v>1</v>
@@ -1633,37 +1660,115 @@
         <v>4</v>
       </c>
       <c r="H33" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="18">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D34" s="6">
+        <v>89.99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>95</v>
+      </c>
+      <c r="F34" s="1">
+        <v>1</v>
+      </c>
+      <c r="G34" s="1">
+        <v>4</v>
+      </c>
+      <c r="H34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="6">
+        <v>48</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="1">
+        <v>1</v>
+      </c>
+      <c r="G35" s="1">
+        <v>4</v>
+      </c>
+      <c r="H35" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>100</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45</v>
+      </c>
+      <c r="E36" t="s">
+        <v>101</v>
+      </c>
+      <c r="F36" s="1">
+        <v>1</v>
+      </c>
+      <c r="G36" s="1">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
         <v>102</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C37" t="s">
         <v>103</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D37" s="6">
         <v>65</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E37" t="s">
         <v>104</v>
       </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1">
-        <v>4</v>
-      </c>
-      <c r="H34" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="D35" s="1"/>
+      <c r="F37" s="1">
+        <v>1</v>
+      </c>
+      <c r="G37" s="1">
+        <v>4</v>
+      </c>
+      <c r="H37" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="D38" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>